<commit_message>
home screen button layout
</commit_message>
<xml_diff>
--- a/tools/localize/localize.xlsx
+++ b/tools/localize/localize.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>STT</t>
   </si>
@@ -109,19 +109,70 @@
   </si>
   <si>
     <t>Account</t>
+  </si>
+  <si>
+    <t>lang_student_traking</t>
+  </si>
+  <si>
+    <t>lang_report_absentee</t>
+  </si>
+  <si>
+    <t>lang_register_service</t>
+  </si>
+  <si>
+    <t>lang_change_or_cancel_service</t>
+  </si>
+  <si>
+    <t>lang_register_guardian</t>
+  </si>
+  <si>
+    <t>THEO DÕI VỊ TRÍ XE</t>
+  </si>
+  <si>
+    <t>BUS LOCATION TRACKING</t>
+  </si>
+  <si>
+    <t>REPORT ABSENTEE</t>
+  </si>
+  <si>
+    <t>REGISTER BUS SERVICE</t>
+  </si>
+  <si>
+    <t>UPDATE BUS SERVICE</t>
+  </si>
+  <si>
+    <t>REGISTER GUARDIANS</t>
+  </si>
+  <si>
+    <t>BÁO NGHỈ CHO CON</t>
+  </si>
+  <si>
+    <t>ĐĂNG KÍ DỊCH VỤ XE BUÝT</t>
+  </si>
+  <si>
+    <t>THAY ĐỔI DỊCH VỤ XE BUÝT</t>
+  </si>
+  <si>
+    <t>ĐĂNG KÍ THÔNG TIN NGƯỜI GIÁM HỘ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -144,8 +195,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,7 +604,63 @@
         <v>29</v>
       </c>
     </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
home:  + event click items grid
</commit_message>
<xml_diff>
--- a/tools/localize/localize.xlsx
+++ b/tools/localize/localize.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>STT</t>
   </si>
@@ -111,9 +111,6 @@
     <t>Account</t>
   </si>
   <si>
-    <t>lang_student_traking</t>
-  </si>
-  <si>
     <t>lang_report_absentee</t>
   </si>
   <si>
@@ -154,6 +151,45 @@
   </si>
   <si>
     <t>ĐĂNG KÍ THÔNG TIN NGƯỜI GIÁM HỘ</t>
+  </si>
+  <si>
+    <t>lang_noti_header</t>
+  </si>
+  <si>
+    <t>Thông Báo!</t>
+  </si>
+  <si>
+    <t>Notification!</t>
+  </si>
+  <si>
+    <t>lang_noti_login</t>
+  </si>
+  <si>
+    <t>Login to continue</t>
+  </si>
+  <si>
+    <t>Bạn cần đăng nhập để tiếp tục</t>
+  </si>
+  <si>
+    <t>lang_confirm_ok</t>
+  </si>
+  <si>
+    <t>Đồng ý</t>
+  </si>
+  <si>
+    <t>Ok</t>
+  </si>
+  <si>
+    <t>lang_confirm_cancel</t>
+  </si>
+  <si>
+    <t>Hủy bỏ</t>
+  </si>
+  <si>
+    <t>Cancel</t>
+  </si>
+  <si>
+    <t>lang_student_tracking</t>
   </si>
 </sst>
 </file>
@@ -481,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,57 +642,101 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>40</v>
+      <c r="B16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
navigate between [login] <=> [home]
</commit_message>
<xml_diff>
--- a/tools/localize/localize.xlsx
+++ b/tools/localize/localize.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="83">
   <si>
     <t>STT</t>
   </si>
@@ -190,6 +190,84 @@
   </si>
   <si>
     <t>lang_student_tracking</t>
+  </si>
+  <si>
+    <t>lang_account</t>
+  </si>
+  <si>
+    <t>Tài khoản</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Mật khẩu</t>
+  </si>
+  <si>
+    <t>lang_password</t>
+  </si>
+  <si>
+    <t>lang_change_password</t>
+  </si>
+  <si>
+    <t>Đổi Mật Khẩu</t>
+  </si>
+  <si>
+    <t>Change Password</t>
+  </si>
+  <si>
+    <t>lang_forget_password</t>
+  </si>
+  <si>
+    <t>Chưa Có/ Quên Mật Khẩu</t>
+  </si>
+  <si>
+    <t>Forget Password</t>
+  </si>
+  <si>
+    <t>lang_phone_number</t>
+  </si>
+  <si>
+    <t>lang_email_receive_password</t>
+  </si>
+  <si>
+    <t>lang_student_code</t>
+  </si>
+  <si>
+    <t>Mã số sinh viên</t>
+  </si>
+  <si>
+    <t>Student ID</t>
+  </si>
+  <si>
+    <t>lang_send_get_login_info</t>
+  </si>
+  <si>
+    <t>Gửi Thông Tin Xác Thực</t>
+  </si>
+  <si>
+    <t>Request Log In Info</t>
+  </si>
+  <si>
+    <t>lang_back_to_login</t>
+  </si>
+  <si>
+    <t>Quay Về Trang Đăng Nhập</t>
+  </si>
+  <si>
+    <t>Back To LogIn Page</t>
+  </si>
+  <si>
+    <t>Số điện thoại</t>
+  </si>
+  <si>
+    <t>Địa chỉ email nhận mật khẩu</t>
+  </si>
+  <si>
+    <t>Phone number</t>
+  </si>
+  <si>
+    <t>Address receive password</t>
   </si>
 </sst>
 </file>
@@ -517,17 +595,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.5703125" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+    <col min="2" max="2" width="42.140625" customWidth="1"/>
+    <col min="3" max="3" width="32.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -554,189 +632,288 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>65</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>68</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>79</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>69</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>80</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>70</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>71</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>73</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>76</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>77</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>35</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>36</v>
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>37</v>
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>38</v>
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>39</v>
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>46</v>
+        <v>21</v>
+      </c>
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>48</v>
+        <v>24</v>
+      </c>
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>50</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B26" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>53</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Method:   + Forget Password
</commit_message>
<xml_diff>
--- a/tools/localize/localize.xlsx
+++ b/tools/localize/localize.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="89">
   <si>
     <t>STT</t>
   </si>
@@ -268,6 +268,24 @@
   </si>
   <si>
     <t>Address receive password</t>
+  </si>
+  <si>
+    <t>lang_type_new_password</t>
+  </si>
+  <si>
+    <t>Mật khẩu mới</t>
+  </si>
+  <si>
+    <t>New password</t>
+  </si>
+  <si>
+    <t>Confirm new password</t>
+  </si>
+  <si>
+    <t>Nhập lại mật khẩu mới</t>
+  </si>
+  <si>
+    <t>lang_confirm_new_password</t>
   </si>
 </sst>
 </file>
@@ -595,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -718,201 +736,223 @@
         <v>78</v>
       </c>
     </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" t="s">
+        <v>85</v>
+      </c>
+    </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>88</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" t="s">
-        <v>14</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C17" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>35</v>
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>36</v>
+        <v>27</v>
+      </c>
+      <c r="B20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>31</v>
+      <c r="A21" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>61</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B31" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>59</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Children tracking:   + update map
</commit_message>
<xml_diff>
--- a/tools/localize/localize.xlsx
+++ b/tools/localize/localize.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="98">
   <si>
     <t>STT</t>
   </si>
@@ -304,6 +304,15 @@
   </si>
   <si>
     <t>On bus</t>
+  </si>
+  <si>
+    <t>lang_bus_transport</t>
+  </si>
+  <si>
+    <t>Xe đưa đón</t>
+  </si>
+  <si>
+    <t>Bus No</t>
   </si>
 </sst>
 </file>
@@ -631,10 +640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -996,6 +1005,17 @@
         <v>94</v>
       </c>
     </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B35" t="s">
+        <v>96</v>
+      </c>
+      <c r="C35" t="s">
+        <v>97</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Report Absence:   + Phase 1
</commit_message>
<xml_diff>
--- a/tools/localize/localize.xlsx
+++ b/tools/localize/localize.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="110">
   <si>
     <t>STT</t>
   </si>
@@ -333,13 +333,22 @@
     <t>lang_map_type_satellite</t>
   </si>
   <si>
-    <t>lang_pick_date</t>
-  </si>
-  <si>
-    <t>Select Date</t>
-  </si>
-  <si>
-    <t>Chọn Thời Gian</t>
+    <t>Chọn</t>
+  </si>
+  <si>
+    <t>lang_select</t>
+  </si>
+  <si>
+    <t>Select</t>
+  </si>
+  <si>
+    <t>lang_report_absence</t>
+  </si>
+  <si>
+    <t>Báo Nghỉ</t>
+  </si>
+  <si>
+    <t>Report Absence</t>
   </si>
 </sst>
 </file>
@@ -667,20 +676,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" customWidth="1"/>
-    <col min="2" max="2" width="42.140625" customWidth="1"/>
-    <col min="3" max="3" width="32.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.5546875" customWidth="1"/>
+    <col min="2" max="2" width="42.109375" customWidth="1"/>
+    <col min="3" max="3" width="32.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -691,7 +700,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -702,7 +711,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -713,7 +722,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>62</v>
       </c>
@@ -724,7 +733,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -735,7 +744,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>65</v>
       </c>
@@ -746,7 +755,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>66</v>
       </c>
@@ -757,7 +766,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>67</v>
       </c>
@@ -768,7 +777,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>70</v>
       </c>
@@ -779,7 +788,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>73</v>
       </c>
@@ -790,7 +799,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>80</v>
       </c>
@@ -801,7 +810,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>85</v>
       </c>
@@ -812,7 +821,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -823,7 +832,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -834,7 +843,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -845,7 +854,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -856,7 +865,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -867,7 +876,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -878,7 +887,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -889,7 +898,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>53</v>
       </c>
@@ -900,7 +909,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -911,7 +920,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -922,7 +931,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -933,7 +942,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -944,7 +953,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>44</v>
       </c>
@@ -955,7 +964,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>46</v>
       </c>
@@ -966,7 +975,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>47</v>
       </c>
@@ -977,7 +986,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>50</v>
       </c>
@@ -988,7 +997,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>54</v>
       </c>
@@ -999,7 +1008,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>58</v>
       </c>
@@ -1010,7 +1019,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>92</v>
       </c>
@@ -1021,7 +1030,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>89</v>
       </c>
@@ -1032,7 +1041,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>95</v>
       </c>
@@ -1043,7 +1052,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>100</v>
       </c>
@@ -1054,7 +1063,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>103</v>
       </c>
@@ -1065,15 +1074,26 @@
         <v>99</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
+        <v>105</v>
+      </c>
+      <c r="B39" t="s">
         <v>104</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
         <v>106</v>
       </c>
-      <c r="C39" t="s">
-        <v>105</v>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>107</v>
+      </c>
+      <c r="B40" t="s">
+        <v>108</v>
+      </c>
+      <c r="C40" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Register Service:   + Search & Select Place
</commit_message>
<xml_diff>
--- a/tools/localize/localize.xlsx
+++ b/tools/localize/localize.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="152">
   <si>
     <t>STT</t>
   </si>
@@ -466,13 +466,22 @@
   </si>
   <si>
     <t>Search Address</t>
+  </si>
+  <si>
+    <t>lang_select_place</t>
+  </si>
+  <si>
+    <t>Chọn Địa Chỉ Này</t>
+  </si>
+  <si>
+    <t>Select This Address</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -490,6 +499,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFCE9178"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -512,12 +527,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -798,10 +816,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C53"/>
+  <dimension ref="A1:C54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1376,6 +1394,17 @@
         <v>148</v>
       </c>
     </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Register Service:   + Change Place By Moving Marker
</commit_message>
<xml_diff>
--- a/tools/localize/localize.xlsx
+++ b/tools/localize/localize.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="155">
   <si>
     <t>STT</t>
   </si>
@@ -475,6 +475,15 @@
   </si>
   <si>
     <t>Select This Address</t>
+  </si>
+  <si>
+    <t>lang_pick_here</t>
+  </si>
+  <si>
+    <t>Đón Tại Đây</t>
+  </si>
+  <si>
+    <t>Pick Here</t>
   </si>
 </sst>
 </file>
@@ -816,10 +825,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C54"/>
+  <dimension ref="A1:C55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1405,6 +1414,17 @@
         <v>151</v>
       </c>
     </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Register Serive:   + Set Start Date
</commit_message>
<xml_diff>
--- a/tools/localize/localize.xlsx
+++ b/tools/localize/localize.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="173">
   <si>
     <t>STT</t>
   </si>
@@ -484,6 +484,60 @@
   </si>
   <si>
     <t>Pick Here</t>
+  </si>
+  <si>
+    <t>lang_next</t>
+  </si>
+  <si>
+    <t>Tiếp Theo</t>
+  </si>
+  <si>
+    <t>Next</t>
+  </si>
+  <si>
+    <t>lang_partner_list</t>
+  </si>
+  <si>
+    <t>Người Đi Cùng</t>
+  </si>
+  <si>
+    <t>Partner</t>
+  </si>
+  <si>
+    <t>lang_pick_method_with_parent</t>
+  </si>
+  <si>
+    <t>Parent go with Student until kick off</t>
+  </si>
+  <si>
+    <t>lang_pick_method_by_student</t>
+  </si>
+  <si>
+    <t>Student kickk off and go off istself</t>
+  </si>
+  <si>
+    <t>PH giao HS tận tay Giám sát Xe</t>
+  </si>
+  <si>
+    <t>HS tự đón xe và về tại điểm đón trả</t>
+  </si>
+  <si>
+    <t>lang_service_start_date</t>
+  </si>
+  <si>
+    <t>Ngày bắt đầu dịch vụ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Service Starting Date </t>
+  </si>
+  <si>
+    <t>lang_alert_wrong_year</t>
+  </si>
+  <si>
+    <t>Vui lòng điều chỉnh năm đăng kí @year@</t>
+  </si>
+  <si>
+    <t>Please adjust Year @year@</t>
   </si>
 </sst>
 </file>
@@ -825,15 +879,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C55"/>
+  <dimension ref="A1:C61"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="1" max="1" width="51.140625" customWidth="1"/>
     <col min="2" max="2" width="42.140625" customWidth="1"/>
     <col min="3" max="3" width="32.7109375" customWidth="1"/>
   </cols>
@@ -1425,6 +1479,72 @@
         <v>154</v>
       </c>
     </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Register Service:   + Complete
</commit_message>
<xml_diff>
--- a/tools/localize/localize.xlsx
+++ b/tools/localize/localize.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="197">
   <si>
     <t>STT</t>
   </si>
@@ -538,6 +538,78 @@
   </si>
   <si>
     <t>Please adjust Year @year@</t>
+  </si>
+  <si>
+    <t>lang_prev</t>
+  </si>
+  <si>
+    <t>Quay Lại</t>
+  </si>
+  <si>
+    <t>Previous</t>
+  </si>
+  <si>
+    <t>lang_select_guardians_max</t>
+  </si>
+  <si>
+    <t>Select @max@ of Guardians</t>
+  </si>
+  <si>
+    <t>lang_confirm</t>
+  </si>
+  <si>
+    <t>Xác Nhận</t>
+  </si>
+  <si>
+    <t>Confirm</t>
+  </si>
+  <si>
+    <t>lang_agree_policy</t>
+  </si>
+  <si>
+    <t>Tôi đã đọc và đồng ý với</t>
+  </si>
+  <si>
+    <t>I have read and agreed with</t>
+  </si>
+  <si>
+    <t>lang_policy</t>
+  </si>
+  <si>
+    <t>Bản Cam Kết</t>
+  </si>
+  <si>
+    <t>Agreement</t>
+  </si>
+  <si>
+    <t>Chọn tối đa @max@ Người Giám hộ</t>
+  </si>
+  <si>
+    <t>lang_please_agree_policy</t>
+  </si>
+  <si>
+    <t>Please agree with Agreement</t>
+  </si>
+  <si>
+    <t>lang_accept</t>
+  </si>
+  <si>
+    <t>Đồng Ý</t>
+  </si>
+  <si>
+    <t>Accept</t>
+  </si>
+  <si>
+    <t>lang_reject</t>
+  </si>
+  <si>
+    <t>Từ Chối</t>
+  </si>
+  <si>
+    <t>Reject</t>
+  </si>
+  <si>
+    <t>Vui lòng đồng ý nội dung Bản cam kết</t>
   </si>
 </sst>
 </file>
@@ -879,10 +951,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C61"/>
+  <dimension ref="A1:C69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+      <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1492,57 +1564,145 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>158</v>
+        <v>173</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>159</v>
+        <v>174</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>160</v>
+        <v>175</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B60" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="C60" s="2" t="s">
         <v>164</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B62" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="C62" s="2" t="s">
         <v>172</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>195</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Register Service:   + Update condition
</commit_message>
<xml_diff>
--- a/tools/localize/localize.xlsx
+++ b/tools/localize/localize.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="206">
   <si>
     <t>STT</t>
   </si>
@@ -619,13 +619,31 @@
   </si>
   <si>
     <t>Get Info Login</t>
+  </si>
+  <si>
+    <t>lang_confirm_register_service_header</t>
+  </si>
+  <si>
+    <t>Xác Nhận Đăng Kí</t>
+  </si>
+  <si>
+    <t>Confirm Register Service</t>
+  </si>
+  <si>
+    <t>lang_confirm_register_service_content</t>
+  </si>
+  <si>
+    <t>Phí dịch vụ xe buýt là @value@ Đồng, bạn có đồng ý đăng kí không ?</t>
+  </si>
+  <si>
+    <t>Service Price is @value@ VND, do you want to register ?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -643,12 +661,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFCE9178"/>
-      <name val="Consolas"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -673,12 +685,14 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -960,769 +974,792 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C70"/>
+  <dimension ref="A1:C72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.140625" customWidth="1"/>
-    <col min="2" max="2" width="42.140625" customWidth="1"/>
-    <col min="3" max="3" width="32.7109375" customWidth="1"/>
+    <col min="1" max="1" width="51.140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="42.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="32.7109375" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="1" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="1" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="1" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="1" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="1" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="1" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" s="1" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+      <c r="A36" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="1" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C37" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C38" s="1" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+      <c r="A40" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" s="1" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+      <c r="A41" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C41" s="1" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+      <c r="A42" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C42" s="1" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+      <c r="A43" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C43" s="1" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+      <c r="A44" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C44" s="1" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+      <c r="A45" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C45" s="1" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+      <c r="A46" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C46" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+    <row r="47" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C47" s="1" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
+      <c r="A48" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B48" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C48" s="1" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+      <c r="A49" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B49" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="C49" s="1" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+      <c r="A50" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B50" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="C50" s="1" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
+      <c r="A51" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B51" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="C51" s="1" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
+      <c r="A52" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B52" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="C52" s="1" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
+      <c r="A53" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B53" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C53" s="1" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
+      <c r="A54" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B54" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="C54" s="1" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
+      <c r="A55" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B55" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="C55" s="1" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
+      <c r="A56" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B56" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="C56" s="1" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
+      <c r="A57" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B57" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="C57" s="1" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
+      <c r="A58" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B58" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="C58" s="1" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
+      <c r="A59" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B59" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="C59" s="1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
+    <row r="60" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B60" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="C60" s="1" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
+      <c r="A61" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B61" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="C61" s="1" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="3" t="s">
+      <c r="A62" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B62" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="C62" s="1" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="3" t="s">
+      <c r="A63" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B63" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="C63" s="1" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
+      <c r="A64" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="B64" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="C64" s="1" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
+      <c r="A65" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B65" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="C65" s="2" t="s">
+      <c r="C65" s="1" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="3" t="s">
+      <c r="A66" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B66" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="C66" s="1" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="3" t="s">
+      <c r="A67" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B67" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="C67" s="1" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="3" t="s">
+      <c r="A68" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B68" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="C68" s="2" t="s">
+      <c r="C68" s="1" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="3" t="s">
+      <c r="A69" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B69" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="C69" s="2" t="s">
+      <c r="C69" s="1" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="3" t="s">
+      <c r="A70" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B70" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="C70" s="2" t="s">
+      <c r="C70" s="1" t="s">
         <v>195</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Register Guardians:   + #1
</commit_message>
<xml_diff>
--- a/tools/localize/localize.xlsx
+++ b/tools/localize/localize.xlsx
@@ -1075,8 +1075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="C81" sqref="C81"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Register Guardian:   + Add guardians
</commit_message>
<xml_diff>
--- a/tools/localize/localize.xlsx
+++ b/tools/localize/localize.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="251">
   <si>
     <t>STT</t>
   </si>
@@ -754,6 +754,24 @@
   </si>
   <si>
     <t>Thêm Giám Hộ</t>
+  </si>
+  <si>
+    <t>lang_select_image</t>
+  </si>
+  <si>
+    <t>Chọn Ảnh</t>
+  </si>
+  <si>
+    <t>Select Image</t>
+  </si>
+  <si>
+    <t>lang_full_name</t>
+  </si>
+  <si>
+    <t>Họ &amp; Tên</t>
+  </si>
+  <si>
+    <t>Full Name</t>
   </si>
 </sst>
 </file>
@@ -1100,10 +1118,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C85"/>
+  <dimension ref="A1:C87"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83"/>
+      <selection activeCell="C87" sqref="C87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2031,6 +2049,28 @@
         <v>241</v>
       </c>
     </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>250</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Guardians:   + Update guardian's info
</commit_message>
<xml_diff>
--- a/tools/localize/localize.xlsx
+++ b/tools/localize/localize.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="260">
   <si>
     <t>STT</t>
   </si>
@@ -772,6 +772,33 @@
   </si>
   <si>
     <t>Full Name</t>
+  </si>
+  <si>
+    <t>lang_edit_guardian</t>
+  </si>
+  <si>
+    <t>Thông Tin Giám Hộ</t>
+  </si>
+  <si>
+    <t>Guardians Info</t>
+  </si>
+  <si>
+    <t>lang_confirm_delete_guardian</t>
+  </si>
+  <si>
+    <t>Xác Nhận Xóa Giám Hộ @guardian@ ?</t>
+  </si>
+  <si>
+    <t>Xác Nhận Cập Nhật Thông Tin Giám Hộ ?</t>
+  </si>
+  <si>
+    <t>Confirm Update Guardian's Info ?</t>
+  </si>
+  <si>
+    <t>Confirm Delete Guardian @guardian@ ?</t>
+  </si>
+  <si>
+    <t>lang_confirm_update_guardian</t>
   </si>
 </sst>
 </file>
@@ -1118,10 +1145,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C87"/>
+  <dimension ref="A1:C90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="C87" sqref="C87"/>
+    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="A90" sqref="A90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2071,6 +2098,39 @@
         <v>250</v>
       </c>
     </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A89" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Account:   + Parent   + Student
</commit_message>
<xml_diff>
--- a/tools/localize/localize.xlsx
+++ b/tools/localize/localize.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="266">
   <si>
     <t>STT</t>
   </si>
@@ -799,6 +799,24 @@
   </si>
   <si>
     <t>lang_confirm_update_guardian</t>
+  </si>
+  <si>
+    <t>lang_parent</t>
+  </si>
+  <si>
+    <t>Phụ Huynh</t>
+  </si>
+  <si>
+    <t>Parent</t>
+  </si>
+  <si>
+    <t>lang_student</t>
+  </si>
+  <si>
+    <t>Học Sinh</t>
+  </si>
+  <si>
+    <t>Student</t>
   </si>
 </sst>
 </file>
@@ -1145,10 +1163,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C90"/>
+  <dimension ref="A1:C92"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="A90" sqref="A90"/>
+      <selection activeCell="C92" sqref="C92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2131,6 +2149,28 @@
         <v>257</v>
       </c>
     </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>265</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Construct Layout multi Screen size:   + History   + Children Tracking   + Report Absence
</commit_message>
<xml_diff>
--- a/tools/localize/localize.xlsx
+++ b/tools/localize/localize.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="276">
   <si>
     <t>STT</t>
   </si>
@@ -123,36 +123,6 @@
     <t>lang_register_guardian</t>
   </si>
   <si>
-    <t>THEO DÕI VỊ TRÍ XE</t>
-  </si>
-  <si>
-    <t>BUS LOCATION TRACKING</t>
-  </si>
-  <si>
-    <t>REPORT ABSENTEE</t>
-  </si>
-  <si>
-    <t>REGISTER BUS SERVICE</t>
-  </si>
-  <si>
-    <t>UPDATE BUS SERVICE</t>
-  </si>
-  <si>
-    <t>REGISTER GUARDIANS</t>
-  </si>
-  <si>
-    <t>BÁO NGHỈ CHO CON</t>
-  </si>
-  <si>
-    <t>ĐĂNG KÍ DỊCH VỤ XE BUÝT</t>
-  </si>
-  <si>
-    <t>THAY ĐỔI DỊCH VỤ XE BUÝT</t>
-  </si>
-  <si>
-    <t>ĐĂNG KÍ THÔNG TIN NGƯỜI GIÁM HỘ</t>
-  </si>
-  <si>
     <t>lang_noti_header</t>
   </si>
   <si>
@@ -817,6 +787,66 @@
   </si>
   <si>
     <t>Student</t>
+  </si>
+  <si>
+    <t>Theo Dõi Vị Trí Xe</t>
+  </si>
+  <si>
+    <t>Bus Location Tracking</t>
+  </si>
+  <si>
+    <t>Report Absence</t>
+  </si>
+  <si>
+    <t>Register Bus Service</t>
+  </si>
+  <si>
+    <t>Update Bus Service</t>
+  </si>
+  <si>
+    <t>Báo Nghỉ Cho Con</t>
+  </si>
+  <si>
+    <t>Đăng Kí Dịch Vụ Xe Buýt</t>
+  </si>
+  <si>
+    <t>Thay Đổi Dịch Vụ Xe Buýt</t>
+  </si>
+  <si>
+    <t>Đăng Kí Thông Tin Giám Hộ</t>
+  </si>
+  <si>
+    <t>Register Guardian</t>
+  </si>
+  <si>
+    <t>lang_student_tracking_des</t>
+  </si>
+  <si>
+    <t>lang_report_absentee_des</t>
+  </si>
+  <si>
+    <t>lang_register_service_des</t>
+  </si>
+  <si>
+    <t>lang_change_or_cancel_service_des</t>
+  </si>
+  <si>
+    <t>lang_register_guardian_des</t>
+  </si>
+  <si>
+    <t>Theo dõi vị trí hiện tại của học sinh, vị trí hiện tại của các chuyến xe buýt đang đến</t>
+  </si>
+  <si>
+    <t>Thông báo nghỉ cho học sinh không sử dụng dịch vụ xe buýt trong 1 khoảng thời gian</t>
+  </si>
+  <si>
+    <t>Đăng kí dịch vụ xe buýt, chọn điểm đón, năm đăng kí, danh sách giám hộ,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thay đổi dịch vụ xe buýt đã đăng kí, </t>
+  </si>
+  <si>
+    <t>Đăng kí thông tin các giám hộ, là người đi cùng học sinh trên xe buýt</t>
   </si>
 </sst>
 </file>
@@ -1163,10 +1193,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C92"/>
+  <dimension ref="A1:C97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="C92" sqref="C92"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28:C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1201,35 +1231,35 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1245,79 +1275,79 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1404,13 +1434,13 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>34</v>
+        <v>256</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>35</v>
+        <v>257</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1418,10 +1448,10 @@
         <v>30</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>40</v>
+        <v>261</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>36</v>
+        <v>258</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1429,10 +1459,10 @@
         <v>31</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>41</v>
+        <v>262</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>37</v>
+        <v>259</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -1440,10 +1470,10 @@
         <v>32</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>42</v>
+        <v>263</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>38</v>
+        <v>260</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -1451,724 +1481,779 @@
         <v>33</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>43</v>
+        <v>264</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>44</v>
+        <v>266</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>86</v>
+        <v>271</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>46</v>
+        <v>267</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>87</v>
+        <v>272</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>47</v>
+        <v>268</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>48</v>
+        <v>273</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>49</v>
+        <v>273</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>50</v>
+        <v>269</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>51</v>
+        <v>274</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>54</v>
+        <v>270</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>55</v>
+        <v>275</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>29</v>
+        <v>275</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
+      <c r="A33" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>92</v>
+        <v>37</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>90</v>
+        <v>38</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>91</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>89</v>
+        <v>40</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>93</v>
+        <v>41</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>94</v>
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>95</v>
+      <c r="A36" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>96</v>
+        <v>45</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>97</v>
+        <v>29</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>100</v>
+        <v>48</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>102</v>
+        <v>47</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>101</v>
+        <v>46</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>99</v>
-      </c>
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
+      <c r="A39" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>105</v>
+        <v>79</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>110</v>
+      <c r="A42" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
-        <v>113</v>
+      <c r="A43" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>117</v>
+        <v>88</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>114</v>
+        <v>89</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>121</v>
-      </c>
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
-        <v>118</v>
+      <c r="A45" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>119</v>
+        <v>94</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>120</v>
+        <v>96</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>122</v>
+        <v>97</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>123</v>
+        <v>98</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>125</v>
+        <v>100</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>126</v>
+        <v>101</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>127</v>
+        <v>102</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>128</v>
+        <v>103</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>130</v>
+        <v>107</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>129</v>
+        <v>104</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>137</v>
+        <v>105</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>138</v>
+        <v>106</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>139</v>
+        <v>111</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>131</v>
+        <v>108</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>134</v>
+        <v>112</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>135</v>
+        <v>113</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>140</v>
+        <v>115</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>141</v>
+        <v>116</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>142</v>
+        <v>117</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>143</v>
+        <v>118</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>144</v>
+        <v>120</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>145</v>
+        <v>119</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>146</v>
+        <v>127</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>147</v>
+        <v>128</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>149</v>
+        <v>121</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>150</v>
+        <v>122</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>152</v>
+        <v>124</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>153</v>
+        <v>125</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>154</v>
+        <v>126</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>155</v>
+        <v>130</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>156</v>
+        <v>131</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>157</v>
+        <v>132</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>173</v>
+        <v>133</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>174</v>
+        <v>134</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>175</v>
+        <v>135</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>158</v>
+        <v>136</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>159</v>
+        <v>137</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>161</v>
+        <v>139</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>165</v>
+        <v>140</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>162</v>
+        <v>141</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>163</v>
+        <v>142</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>166</v>
+        <v>143</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>164</v>
+        <v>144</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>167</v>
+        <v>145</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>168</v>
+        <v>146</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>169</v>
+        <v>147</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>176</v>
+        <v>148</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>187</v>
+        <v>149</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>178</v>
+        <v>151</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>180</v>
+        <v>152</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>181</v>
+        <v>153</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>182</v>
+        <v>156</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>183</v>
+        <v>154</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>184</v>
+        <v>157</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>185</v>
+        <v>158</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>186</v>
+        <v>159</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>196</v>
+        <v>161</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>189</v>
+        <v>162</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>190</v>
+        <v>166</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>192</v>
+        <v>167</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>193</v>
+        <v>168</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>194</v>
+        <v>169</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>195</v>
+        <v>170</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>200</v>
+        <v>171</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>201</v>
+        <v>172</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>203</v>
+        <v>174</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>204</v>
+        <v>175</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>205</v>
+        <v>176</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="B73" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>208</v>
+      <c r="A73" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="C74" s="3" t="s">
-        <v>211</v>
+      <c r="A74" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>212</v>
+        <v>183</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>214</v>
+        <v>184</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>213</v>
+        <v>190</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>216</v>
+        <v>191</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>218</v>
+        <v>193</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>220</v>
+        <v>194</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A78" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>222</v>
+        <v>195</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>224</v>
+        <v>199</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>225</v>
+        <v>200</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>226</v>
+        <v>201</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="B80" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>235</v>
+      <c r="A80" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="B82" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="C82" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="4" t="s">
-        <v>236</v>
-      </c>
-      <c r="B83" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="C83" s="3" t="s">
-        <v>237</v>
+      <c r="A82" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A83" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
-        <v>238</v>
+        <v>214</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>239</v>
+        <v>215</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>240</v>
+        <v>216</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
-        <v>243</v>
+        <v>219</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>242</v>
+        <v>217</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="4" t="s">
-        <v>245</v>
+      <c r="A86" s="3" t="s">
+        <v>220</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>246</v>
+        <v>224</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>247</v>
+        <v>225</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="3" t="s">
-        <v>248</v>
+      <c r="A87" s="4" t="s">
+        <v>221</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>249</v>
+        <v>223</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>250</v>
+        <v>222</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
-        <v>251</v>
+        <v>226</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>252</v>
+        <v>234</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
-        <v>254</v>
+        <v>228</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>255</v>
+        <v>229</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>258</v>
+        <v>230</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
-        <v>259</v>
+        <v>233</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>256</v>
+        <v>232</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>257</v>
+        <v>231</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="3" t="s">
-        <v>260</v>
+      <c r="A91" s="4" t="s">
+        <v>235</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>261</v>
+        <v>236</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>262</v>
+        <v>237</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
-        <v>263</v>
+        <v>238</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>264</v>
+        <v>239</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>265</v>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A94" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>255</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Construct Layout multi Screen size:  + Change Service
</commit_message>
<xml_diff>
--- a/tools/localize/localize.xlsx
+++ b/tools/localize/localize.xlsx
@@ -1195,8 +1195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28:C31"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Construct Layout multi Screen size:  + Log In
</commit_message>
<xml_diff>
--- a/tools/localize/localize.xlsx
+++ b/tools/localize/localize.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="282">
   <si>
     <t>STT</t>
   </si>
@@ -847,13 +847,31 @@
   </si>
   <si>
     <t>Đăng kí thông tin các giám hộ, là người đi cùng học sinh trên xe buýt</t>
+  </si>
+  <si>
+    <t>lang_log_out</t>
+  </si>
+  <si>
+    <t>Đăng Xuất</t>
+  </si>
+  <si>
+    <t>Log Out</t>
+  </si>
+  <si>
+    <t>lang_confirm_log_out</t>
+  </si>
+  <si>
+    <t>Are You Sure Log Out ?</t>
+  </si>
+  <si>
+    <t>Xác Nhận Thoát Đăng Nhập Tài Khoản ?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -871,12 +889,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFCE9178"/>
-      <name val="Consolas"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -910,7 +922,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1193,10 +1205,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C97"/>
+  <dimension ref="A1:C99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="A78" sqref="A78"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2040,21 +2052,21 @@
       <c r="A78" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="B78" s="3" t="s">
+      <c r="B78" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="C78" s="3" t="s">
+      <c r="C78" s="1" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="3" t="s">
+      <c r="A79" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="B79" s="3" t="s">
+      <c r="B79" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="C79" s="3" t="s">
+      <c r="C79" s="1" t="s">
         <v>201</v>
       </c>
     </row>
@@ -2103,35 +2115,35 @@
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="3" t="s">
+      <c r="A84" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="B84" s="3" t="s">
+      <c r="B84" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="C84" s="3" t="s">
+      <c r="C84" s="1" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="3" t="s">
+      <c r="A85" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="B85" s="3" t="s">
+      <c r="B85" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="C85" s="3" t="s">
+      <c r="C85" s="1" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="3" t="s">
+      <c r="A86" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="B86" s="3" t="s">
+      <c r="B86" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="C86" s="3" t="s">
+      <c r="C86" s="1" t="s">
         <v>225</v>
       </c>
     </row>
@@ -2139,10 +2151,10 @@
       <c r="A87" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="B87" s="3" t="s">
+      <c r="B87" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="C87" s="3" t="s">
+      <c r="C87" s="1" t="s">
         <v>222</v>
       </c>
     </row>
@@ -2150,32 +2162,32 @@
       <c r="A88" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="B88" s="3" t="s">
+      <c r="B88" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="C88" s="3" t="s">
+      <c r="C88" s="1" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="3" t="s">
+      <c r="A89" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="B89" s="3" t="s">
+      <c r="B89" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="C89" s="3" t="s">
+      <c r="C89" s="1" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="3" t="s">
+      <c r="A90" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="B90" s="3" t="s">
+      <c r="B90" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="C90" s="3" t="s">
+      <c r="C90" s="1" t="s">
         <v>231</v>
       </c>
     </row>
@@ -2183,21 +2195,21 @@
       <c r="A91" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="B91" s="3" t="s">
+      <c r="B91" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="C91" s="3" t="s">
+      <c r="C91" s="1" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="3" t="s">
+      <c r="A92" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="B92" s="3" t="s">
+      <c r="B92" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="C92" s="3" t="s">
+      <c r="C92" s="1" t="s">
         <v>240</v>
       </c>
     </row>
@@ -2205,55 +2217,77 @@
       <c r="A93" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="B93" s="3" t="s">
+      <c r="B93" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="C93" s="3" t="s">
+      <c r="C93" s="1" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A94" s="3" t="s">
+      <c r="A94" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="B94" s="3" t="s">
+      <c r="B94" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="C94" s="3" t="s">
+      <c r="C94" s="1" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" s="3" t="s">
+      <c r="A95" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="B95" s="3" t="s">
+      <c r="B95" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="C95" s="3" t="s">
+      <c r="C95" s="1" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="3" t="s">
+      <c r="A96" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="B96" s="3" t="s">
+      <c r="B96" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="C96" s="3" t="s">
+      <c r="C96" s="1" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" s="3" t="s">
+      <c r="A97" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="B97" s="3" t="s">
+      <c r="B97" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="C97" s="3" t="s">
+      <c r="C97" s="1" t="s">
         <v>255</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>280</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Compose Mail -> Add to Sent Mail
</commit_message>
<xml_diff>
--- a/tools/localize/localize.xlsx
+++ b/tools/localize/localize.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="288">
   <si>
     <t>STT</t>
   </si>
@@ -865,6 +865,24 @@
   </si>
   <si>
     <t>Xác Nhận Thoát Đăng Nhập Tài Khoản ?</t>
+  </si>
+  <si>
+    <t>lang_blank_history</t>
+  </si>
+  <si>
+    <t>Lịch Sử Trống</t>
+  </si>
+  <si>
+    <t>lang_record</t>
+  </si>
+  <si>
+    <t>_from_ đến _to_</t>
+  </si>
+  <si>
+    <t>_from_  to  _to_</t>
+  </si>
+  <si>
+    <t>History Is Empty</t>
   </si>
 </sst>
 </file>
@@ -911,7 +929,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -924,6 +942,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1205,10 +1226,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C99"/>
+  <dimension ref="A1:C102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="C101" sqref="C101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2290,6 +2311,28 @@
         <v>280</v>
       </c>
     </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="B102" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>286</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Move module change password to Parent Tabs: change password requires log in
</commit_message>
<xml_diff>
--- a/tools/localize/localize.xlsx
+++ b/tools/localize/localize.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="293">
   <si>
     <t>STT</t>
   </si>
@@ -861,9 +861,6 @@
     <t>lang_confirm_log_out</t>
   </si>
   <si>
-    <t>Are You Sure Log Out ?</t>
-  </si>
-  <si>
     <t>Xác Nhận Thoát Đăng Nhập Tài Khoản ?</t>
   </si>
   <si>
@@ -883,6 +880,24 @@
   </si>
   <si>
     <t>History Is Empty</t>
+  </si>
+  <si>
+    <t>Are You Sure To Log Out ?</t>
+  </si>
+  <si>
+    <t>Day off announcement to students</t>
+  </si>
+  <si>
+    <t>Track the current location of students, bus comings</t>
+  </si>
+  <si>
+    <t>Register the bus service, select the place, year, list of gủadians</t>
+  </si>
+  <si>
+    <t>Change the register of bus service</t>
+  </si>
+  <si>
+    <t>Register of guardians, who go with student on bus</t>
   </si>
 </sst>
 </file>
@@ -1228,8 +1243,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="C101" sqref="C101"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1520,7 +1535,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>266</v>
       </c>
@@ -1528,10 +1543,10 @@
         <v>271</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>267</v>
       </c>
@@ -1539,10 +1554,10 @@
         <v>272</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>268</v>
       </c>
@@ -1550,7 +1565,7 @@
         <v>273</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>273</v>
+        <v>290</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1561,7 +1576,7 @@
         <v>274</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>274</v>
+        <v>291</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1572,7 +1587,7 @@
         <v>275</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>275</v>
+        <v>292</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -2305,32 +2320,32 @@
         <v>279</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="B101" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="B101" s="3" t="s">
-        <v>283</v>
-      </c>
       <c r="C101" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="B102" s="5" t="s">
         <v>284</v>
       </c>
-      <c r="B102" s="5" t="s">
+      <c r="C102" s="3" t="s">
         <v>285</v>
-      </c>
-      <c r="C102" s="3" t="s">
-        <v>286</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Children Tracking:   + Switch map typ -> Switch pick type
</commit_message>
<xml_diff>
--- a/tools/localize/localize.xlsx
+++ b/tools/localize/localize.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="297">
   <si>
     <t>STT</t>
   </si>
@@ -898,6 +898,18 @@
   </si>
   <si>
     <t>Register of guardians, who go with student on bus</t>
+  </si>
+  <si>
+    <t>lang_pick_type_UP</t>
+  </si>
+  <si>
+    <t>Pick Up</t>
+  </si>
+  <si>
+    <t>Drop Down</t>
+  </si>
+  <si>
+    <t>lang_pick_type_DOWN</t>
   </si>
 </sst>
 </file>
@@ -1241,10 +1253,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C102"/>
+  <dimension ref="A1:C105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="A105" sqref="A105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2348,6 +2360,28 @@
         <v>285</v>
       </c>
     </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>295</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Mail:   + Read Mail   + Delete Mail
</commit_message>
<xml_diff>
--- a/tools/localize/localize.xlsx
+++ b/tools/localize/localize.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="306">
   <si>
     <t>STT</t>
   </si>
@@ -919,6 +919,24 @@
   </si>
   <si>
     <t>Số hiệu học sinh</t>
+  </si>
+  <si>
+    <t>lang_close</t>
+  </si>
+  <si>
+    <t>Đóng</t>
+  </si>
+  <si>
+    <t>Close</t>
+  </si>
+  <si>
+    <t>lang_confirm_delete_mail</t>
+  </si>
+  <si>
+    <t>Xác nhận xóa thư ?</t>
+  </si>
+  <si>
+    <t>Confirm delete Mail ?</t>
   </si>
 </sst>
 </file>
@@ -1262,10 +1280,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C106"/>
+  <dimension ref="A1:C109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
+      <selection activeCell="C109" sqref="C109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2260,146 +2278,168 @@
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="4" t="s">
+      <c r="A92" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="B92" s="1" t="s">
+      <c r="B93" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="C92" s="1" t="s">
+      <c r="C93" s="1" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="B93" s="1" t="s">
+      <c r="B94" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="C93" s="1" t="s">
+      <c r="C94" s="1" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="4" t="s">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="B94" s="1" t="s">
+      <c r="B95" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="C94" s="1" t="s">
+      <c r="C95" s="1" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
+    <row r="96" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="B95" s="1" t="s">
+      <c r="B96" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="C95" s="1" t="s">
+      <c r="C96" s="1" t="s">
         <v>247</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="B99" s="1" t="s">
+      <c r="B100" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="C99" s="1" t="s">
+      <c r="C100" s="1" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="4" t="s">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="B100" s="1" t="s">
+      <c r="B101" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="C100" s="1" t="s">
+      <c r="C101" s="1" t="s">
         <v>286</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="B102" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="C102" s="3" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="B103" s="5" t="s">
+      <c r="B104" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="C103" s="3" t="s">
+      <c r="C104" s="3" t="s">
         <v>284</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" s="3" t="s">
-        <v>292</v>
-      </c>
-      <c r="B105" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C105" s="3" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="B106" s="3" t="s">
+      <c r="B107" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C106" s="3" t="s">
+      <c r="C107" s="3" t="s">
         <v>294</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="B109" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="C109" s="3" t="s">
+        <v>305</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Children Tracking:   + Multi Child   + Add bus info
</commit_message>
<xml_diff>
--- a/tools/localize/localize.xlsx
+++ b/tools/localize/localize.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="321">
   <si>
     <t>STT</t>
   </si>
@@ -937,13 +937,58 @@
   </si>
   <si>
     <t>Confirm delete Mail ?</t>
+  </si>
+  <si>
+    <t>lang_bus_name</t>
+  </si>
+  <si>
+    <t>Tên tuyến</t>
+  </si>
+  <si>
+    <t>Bus's name</t>
+  </si>
+  <si>
+    <t>lang_bks</t>
+  </si>
+  <si>
+    <t>Biển Kiểm Soát</t>
+  </si>
+  <si>
+    <t>Number Plate</t>
+  </si>
+  <si>
+    <t>lang_driver</t>
+  </si>
+  <si>
+    <t>Driver</t>
+  </si>
+  <si>
+    <t>lang_monitor</t>
+  </si>
+  <si>
+    <t>Tài Xế</t>
+  </si>
+  <si>
+    <t>Giám Sát</t>
+  </si>
+  <si>
+    <t>Monitor</t>
+  </si>
+  <si>
+    <t>lang_time_bus_pick</t>
+  </si>
+  <si>
+    <t>Giờ Đón Trả</t>
+  </si>
+  <si>
+    <t>Pick Time</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -961,6 +1006,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFCE9178"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -983,7 +1034,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -999,6 +1050,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1280,10 +1334,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C109"/>
+  <dimension ref="A1:C115"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="C109" sqref="C109"/>
+      <selection activeCell="C115" sqref="C115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2442,6 +2496,61 @@
         <v>305</v>
       </c>
     </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="C111" s="3" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="B115" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="C115" s="3" t="s">
+        <v>320</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Add multi Child to:   + History
</commit_message>
<xml_diff>
--- a/tools/localize/localize.xlsx
+++ b/tools/localize/localize.xlsx
@@ -1336,8 +1336,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="C115" sqref="C115"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="A116" sqref="A116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Compose Mail:   + Send School   + Send Monitor
</commit_message>
<xml_diff>
--- a/tools/localize/localize.xlsx
+++ b/tools/localize/localize.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="326">
   <si>
     <t>STT</t>
   </si>
@@ -982,6 +982,21 @@
   </si>
   <si>
     <t>Pick Time</t>
+  </si>
+  <si>
+    <t>lang_mail_send_school</t>
+  </si>
+  <si>
+    <t>Gửi Nhà Trường</t>
+  </si>
+  <si>
+    <t>To School</t>
+  </si>
+  <si>
+    <t>lang_pick_up</t>
+  </si>
+  <si>
+    <t>lang_drop_down</t>
   </si>
 </sst>
 </file>
@@ -1334,10 +1349,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C115"/>
+  <dimension ref="A1:C118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="A116" sqref="A116"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="C118" sqref="C118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2551,6 +2566,39 @@
         <v>320</v>
       </c>
     </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="C116" s="3" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="B117" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C117" s="3" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C118" s="3" t="s">
+        <v>294</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Account Info:   + Add multi Child   + Select Guardian on each child
</commit_message>
<xml_diff>
--- a/tools/localize/localize.xlsx
+++ b/tools/localize/localize.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="338">
   <si>
     <t>STT</t>
   </si>
@@ -997,6 +997,42 @@
   </si>
   <si>
     <t>lang_drop_down</t>
+  </si>
+  <si>
+    <t>lang_phone_number_collapse</t>
+  </si>
+  <si>
+    <t>SDT</t>
+  </si>
+  <si>
+    <t>Phone.No</t>
+  </si>
+  <si>
+    <t>lang_phone_number_expand</t>
+  </si>
+  <si>
+    <t>Số Điện Thoại</t>
+  </si>
+  <si>
+    <t>Phone Number</t>
+  </si>
+  <si>
+    <t>lang_role</t>
+  </si>
+  <si>
+    <t>Vai Trò</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>lang_guardians_list</t>
+  </si>
+  <si>
+    <t>Danh Sách Giám Hộ</t>
+  </si>
+  <si>
+    <t>Guardians List</t>
   </si>
 </sst>
 </file>
@@ -1349,10 +1385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C118"/>
+  <dimension ref="A1:C122"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="C118" sqref="C118"/>
+      <selection activeCell="C122" sqref="C122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2599,6 +2635,50 @@
         <v>294</v>
       </c>
     </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="B119" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="C119" s="3" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="C120" s="3" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="B121" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="C121" s="3" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="B122" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="C122" s="3" t="s">
+        <v>337</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Child Info:   + Add Child Detail
</commit_message>
<xml_diff>
--- a/tools/localize/localize.xlsx
+++ b/tools/localize/localize.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="373">
   <si>
     <t>STT</t>
   </si>
@@ -1033,6 +1033,111 @@
   </si>
   <si>
     <t>Guardians List</t>
+  </si>
+  <si>
+    <t>lang_child_info</t>
+  </si>
+  <si>
+    <t>Thông Tin Học Sinh</t>
+  </si>
+  <si>
+    <t>Student Info</t>
+  </si>
+  <si>
+    <t>lang_grade</t>
+  </si>
+  <si>
+    <t>Khối</t>
+  </si>
+  <si>
+    <t>Grade</t>
+  </si>
+  <si>
+    <t>lang_school_place</t>
+  </si>
+  <si>
+    <t>Place</t>
+  </si>
+  <si>
+    <t>lang_pick_header</t>
+  </si>
+  <si>
+    <t>Pick Up/ Drop Down Method</t>
+  </si>
+  <si>
+    <t>lang_pick_place</t>
+  </si>
+  <si>
+    <t>Pick Up Place</t>
+  </si>
+  <si>
+    <t>lang_pick_time_estimate</t>
+  </si>
+  <si>
+    <t>Thời gian đón dự kiến</t>
+  </si>
+  <si>
+    <t>Địa chỉ đón (Điểm đón)</t>
+  </si>
+  <si>
+    <t>Cơ sở học</t>
+  </si>
+  <si>
+    <t>Hình thức đón trả</t>
+  </si>
+  <si>
+    <t>Pick up time (Estimate)</t>
+  </si>
+  <si>
+    <t>lang_drop_place</t>
+  </si>
+  <si>
+    <t>Địa chỉ trả (Điểm trả)</t>
+  </si>
+  <si>
+    <t>Drop Down Place</t>
+  </si>
+  <si>
+    <t>lang_drop_time_estimate</t>
+  </si>
+  <si>
+    <t>Thời gian trả dự kiến</t>
+  </si>
+  <si>
+    <t>Drop down time (Estimate)</t>
+  </si>
+  <si>
+    <t>lang_bus_id</t>
+  </si>
+  <si>
+    <t>Tuyến số</t>
+  </si>
+  <si>
+    <t>Bus Id</t>
+  </si>
+  <si>
+    <t>lang_driver_phone</t>
+  </si>
+  <si>
+    <t>Drives's phone</t>
+  </si>
+  <si>
+    <t>lang_monitor_phone</t>
+  </si>
+  <si>
+    <t>Điện thoại giám sát xe</t>
+  </si>
+  <si>
+    <t>Monitor's phone</t>
+  </si>
+  <si>
+    <t>lang_start_date_service</t>
+  </si>
+  <si>
+    <t>Start of Date service</t>
+  </si>
+  <si>
+    <t>Điện thoại tài xế</t>
   </si>
 </sst>
 </file>
@@ -1385,10 +1490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C122"/>
+  <dimension ref="A1:C134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="C122" sqref="C122"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2679,6 +2784,138 @@
         <v>337</v>
       </c>
     </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" s="6" t="s">
+        <v>338</v>
+      </c>
+      <c r="B123" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="C123" s="3" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="C124" s="3" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="B125" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="C125" s="3" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="C126" s="3" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="B127" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="C127" s="3" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="C128" s="3" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="B129" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="C129" s="3" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="B130" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="C130" s="3" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="B131" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="C131" s="3" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="B132" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="C132" s="3" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="B133" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="C133" s="3" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="B134" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C134" s="3" t="s">
+        <v>371</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
use global authen data
</commit_message>
<xml_diff>
--- a/tools/localize/localize.xlsx
+++ b/tools/localize/localize.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="376">
   <si>
     <t>STT</t>
   </si>
@@ -1138,6 +1138,15 @@
   </si>
   <si>
     <t>Điện thoại tài xế</t>
+  </si>
+  <si>
+    <t>lang_noti_fill</t>
+  </si>
+  <si>
+    <t>Vui lòng điền thông tin hợp lệ</t>
+  </si>
+  <si>
+    <t>Please fill correctly</t>
   </si>
 </sst>
 </file>
@@ -1490,10 +1499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C134"/>
+  <dimension ref="A1:C136"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="C136" sqref="C136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2916,6 +2925,17 @@
         <v>371</v>
       </c>
     </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="B136" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="C136" s="3" t="s">
+        <v>375</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Add view Tracking Save access token
</commit_message>
<xml_diff>
--- a/tools/localize/localize.xlsx
+++ b/tools/localize/localize.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F873676-91C3-43FD-B916-C3AC7DC69D1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9391A54-AF10-4C71-AD37-A7E412CC9052}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="385">
   <si>
     <t>STT</t>
   </si>
@@ -1157,6 +1157,24 @@
   </si>
   <si>
     <t>Connection interupted</t>
+  </si>
+  <si>
+    <t>lang_place_pick_delivery</t>
+  </si>
+  <si>
+    <t>Điểm đón/ trả</t>
+  </si>
+  <si>
+    <t>Place Pick Up/ Delivery</t>
+  </si>
+  <si>
+    <t>lang_check_in</t>
+  </si>
+  <si>
+    <t>Điểm dừng</t>
+  </si>
+  <si>
+    <t>Check In</t>
   </si>
 </sst>
 </file>
@@ -1509,21 +1527,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C138"/>
+  <dimension ref="A1:C139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A126" workbookViewId="0">
-      <selection activeCell="A138" sqref="A138"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="A107" sqref="A107"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="42.109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="32.6640625" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="9.109375" style="3"/>
+    <col min="1" max="1" width="51.140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="42.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="32.7109375" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1534,7 +1552,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1545,7 +1563,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>48</v>
       </c>
@@ -1556,7 +1574,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>51</v>
       </c>
@@ -1567,7 +1585,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>185</v>
       </c>
@@ -1578,7 +1596,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -1589,7 +1607,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>54</v>
       </c>
@@ -1600,7 +1618,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>55</v>
       </c>
@@ -1611,7 +1629,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>56</v>
       </c>
@@ -1622,7 +1640,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>58</v>
       </c>
@@ -1633,7 +1651,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>61</v>
       </c>
@@ -1644,7 +1662,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>68</v>
       </c>
@@ -1655,7 +1673,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>73</v>
       </c>
@@ -1666,12 +1684,12 @@
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>9</v>
       </c>
@@ -1682,7 +1700,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
@@ -1693,7 +1711,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -1704,7 +1722,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
@@ -1715,7 +1733,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
@@ -1726,7 +1744,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
@@ -1737,7 +1755,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>26</v>
       </c>
@@ -1748,7 +1766,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>42</v>
       </c>
@@ -1759,7 +1777,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>29</v>
       </c>
@@ -1770,7 +1788,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
@@ -1781,7 +1799,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>31</v>
       </c>
@@ -1792,7 +1810,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>32</v>
       </c>
@@ -1803,7 +1821,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>258</v>
       </c>
@@ -1814,7 +1832,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>259</v>
       </c>
@@ -1825,7 +1843,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>260</v>
       </c>
@@ -1836,7 +1854,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>261</v>
       </c>
@@ -1847,7 +1865,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>262</v>
       </c>
@@ -1858,7 +1876,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>33</v>
       </c>
@@ -1869,7 +1887,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>35</v>
       </c>
@@ -1880,7 +1898,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>36</v>
       </c>
@@ -1891,7 +1909,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>39</v>
       </c>
@@ -1902,7 +1920,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>43</v>
       </c>
@@ -1913,7 +1931,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>47</v>
       </c>
@@ -1924,12 +1942,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>80</v>
       </c>
@@ -1940,7 +1958,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>77</v>
       </c>
@@ -1951,7 +1969,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>83</v>
       </c>
@@ -1962,7 +1980,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>88</v>
       </c>
@@ -1973,7 +1991,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>91</v>
       </c>
@@ -1984,12 +2002,12 @@
         <v>87</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>93</v>
       </c>
@@ -2000,7 +2018,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>95</v>
       </c>
@@ -2011,7 +2029,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>98</v>
       </c>
@@ -2022,7 +2040,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>289</v>
       </c>
@@ -2033,7 +2051,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>101</v>
       </c>
@@ -2044,7 +2062,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>103</v>
       </c>
@@ -2055,7 +2073,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>106</v>
       </c>
@@ -2066,7 +2084,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>110</v>
       </c>
@@ -2077,7 +2095,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>113</v>
       </c>
@@ -2088,7 +2106,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>116</v>
       </c>
@@ -2099,7 +2117,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>125</v>
       </c>
@@ -2110,7 +2128,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>119</v>
       </c>
@@ -2121,7 +2139,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>122</v>
       </c>
@@ -2132,7 +2150,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>128</v>
       </c>
@@ -2143,7 +2161,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>131</v>
       </c>
@@ -2154,7 +2172,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>134</v>
       </c>
@@ -2165,7 +2183,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>137</v>
       </c>
@@ -2176,7 +2194,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>140</v>
       </c>
@@ -2187,7 +2205,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>143</v>
       </c>
@@ -2198,7 +2216,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>161</v>
       </c>
@@ -2209,7 +2227,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>146</v>
       </c>
@@ -2220,7 +2238,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>149</v>
       </c>
@@ -2231,7 +2249,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>151</v>
       </c>
@@ -2242,7 +2260,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>155</v>
       </c>
@@ -2253,7 +2271,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>158</v>
       </c>
@@ -2264,7 +2282,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>164</v>
       </c>
@@ -2275,7 +2293,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>166</v>
       </c>
@@ -2286,7 +2304,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>169</v>
       </c>
@@ -2297,7 +2315,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>172</v>
       </c>
@@ -2308,7 +2326,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>176</v>
       </c>
@@ -2319,7 +2337,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>178</v>
       </c>
@@ -2330,7 +2348,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>181</v>
       </c>
@@ -2341,7 +2359,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>188</v>
       </c>
@@ -2352,7 +2370,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>191</v>
       </c>
@@ -2363,7 +2381,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>194</v>
       </c>
@@ -2374,7 +2392,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>197</v>
       </c>
@@ -2385,7 +2403,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>200</v>
       </c>
@@ -2396,7 +2414,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>201</v>
       </c>
@@ -2407,7 +2425,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>206</v>
       </c>
@@ -2418,7 +2436,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>207</v>
       </c>
@@ -2429,7 +2447,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>212</v>
       </c>
@@ -2440,7 +2458,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>213</v>
       </c>
@@ -2451,7 +2469,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>214</v>
       </c>
@@ -2462,7 +2480,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
         <v>215</v>
       </c>
@@ -2473,7 +2491,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
         <v>218</v>
       </c>
@@ -2484,7 +2502,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>220</v>
       </c>
@@ -2495,7 +2513,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>225</v>
       </c>
@@ -2506,7 +2524,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>293</v>
       </c>
@@ -2517,7 +2535,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
         <v>227</v>
       </c>
@@ -2528,7 +2546,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>230</v>
       </c>
@@ -2539,7 +2557,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
         <v>233</v>
       </c>
@@ -2550,7 +2568,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>236</v>
       </c>
@@ -2561,7 +2579,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>241</v>
       </c>
@@ -2572,7 +2590,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>242</v>
       </c>
@@ -2583,7 +2601,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>245</v>
       </c>
@@ -2594,7 +2612,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>268</v>
       </c>
@@ -2605,7 +2623,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
         <v>271</v>
       </c>
@@ -2616,7 +2634,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
         <v>273</v>
       </c>
@@ -2627,7 +2645,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
         <v>275</v>
       </c>
@@ -2638,7 +2656,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
         <v>285</v>
       </c>
@@ -2649,7 +2667,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
         <v>288</v>
       </c>
@@ -2660,7 +2678,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
         <v>296</v>
       </c>
@@ -2671,7 +2689,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="6" t="s">
         <v>299</v>
       </c>
@@ -2682,7 +2700,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="6" t="s">
         <v>302</v>
       </c>
@@ -2693,7 +2711,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="6" t="s">
         <v>305</v>
       </c>
@@ -2704,7 +2722,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="6" t="s">
         <v>307</v>
       </c>
@@ -2715,7 +2733,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="6" t="s">
         <v>311</v>
       </c>
@@ -2726,7 +2744,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
         <v>314</v>
       </c>
@@ -2737,7 +2755,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
         <v>317</v>
       </c>
@@ -2748,7 +2766,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
         <v>318</v>
       </c>
@@ -2759,7 +2777,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
         <v>319</v>
       </c>
@@ -2770,7 +2788,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
         <v>322</v>
       </c>
@@ -2781,7 +2799,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
         <v>325</v>
       </c>
@@ -2792,7 +2810,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="6" t="s">
         <v>328</v>
       </c>
@@ -2803,7 +2821,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="6" t="s">
         <v>331</v>
       </c>
@@ -2814,7 +2832,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
         <v>334</v>
       </c>
@@ -2825,7 +2843,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
         <v>337</v>
       </c>
@@ -2836,7 +2854,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
         <v>339</v>
       </c>
@@ -2847,7 +2865,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
         <v>341</v>
       </c>
@@ -2858,7 +2876,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
         <v>343</v>
       </c>
@@ -2869,7 +2887,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
         <v>349</v>
       </c>
@@ -2880,7 +2898,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
         <v>352</v>
       </c>
@@ -2891,7 +2909,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
         <v>355</v>
       </c>
@@ -2902,7 +2920,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
         <v>358</v>
       </c>
@@ -2913,7 +2931,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
         <v>360</v>
       </c>
@@ -2924,7 +2942,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
         <v>363</v>
       </c>
@@ -2935,25 +2953,47 @@
         <v>364</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="B135" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="C135" s="3" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="B136" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="C136" s="3" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" s="3" t="s">
         <v>366</v>
       </c>
-      <c r="B136" s="3" t="s">
+      <c r="B137" s="3" t="s">
         <v>367</v>
       </c>
-      <c r="C136" s="3" t="s">
+      <c r="C137" s="3" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A138" s="3" t="s">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" s="3" t="s">
         <v>376</v>
       </c>
-      <c r="B138" s="3" t="s">
+      <c r="B139" s="3" t="s">
         <v>377</v>
       </c>
-      <c r="C138" s="3" t="s">
+      <c r="C139" s="3" t="s">
         <v>378</v>
       </c>
     </row>

</xml_diff>

<commit_message>
remove service update service
</commit_message>
<xml_diff>
--- a/tools/localize/localize.xlsx
+++ b/tools/localize/localize.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{664BF781-D909-4838-B1D2-D972DA5ABC7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D8B4EB7-2FBB-4769-A514-AFE7CBF033D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="407">
   <si>
     <t>STT</t>
   </si>
@@ -1232,6 +1232,15 @@
   </si>
   <si>
     <t>You have @num@ new mails, please check out</t>
+  </si>
+  <si>
+    <t>lang_remove_service_success</t>
+  </si>
+  <si>
+    <t>Hủy dịch vụ thành công</t>
+  </si>
+  <si>
+    <t>Remove service success</t>
   </si>
 </sst>
 </file>
@@ -1584,10 +1593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C145"/>
+  <dimension ref="A1:C146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
-      <selection activeCell="C145" sqref="C145"/>
+    <sheetView tabSelected="1" topLeftCell="A138" workbookViewId="0">
+      <selection activeCell="C146" sqref="C146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3120,6 +3129,17 @@
         <v>403</v>
       </c>
     </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" s="3" t="s">
+        <v>404</v>
+      </c>
+      <c r="B146" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="C146" s="3" t="s">
+        <v>406</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>